<commit_message>
Modified the resource for Asset services
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/CollectionsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">cheque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state bank of india</t>
   </si>
   <si>
     <t xml:space="preserve">dd</t>
@@ -275,11 +278,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,13 +337,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,17 +416,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.8777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,17 +475,17 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,8 +523,8 @@
       <c r="B3" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>102</v>
+      <c r="C3" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>30</v>
@@ -529,13 +532,13 @@
     </row>
     <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>102</v>
+      <c r="C4" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>30</v>
@@ -543,32 +546,32 @@
     </row>
     <row r="5" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>123456</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>123987</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>844810206002</v>

</xml_diff>